<commit_message>
Added more EDA on monthly loan amounts
</commit_message>
<xml_diff>
--- a/dataDefs/datasets_34_1110834_LCDataDictionary.xlsx
+++ b/dataDefs/datasets_34_1110834_LCDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simondyates/Dropbox/DataSci/PycharmProjects/Lending-Club/dataDefs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F229E2A-BF9D-CF4A-9B01-753C6D4AA774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA6AFA0-23DD-A144-884A-7A5EB21B3EC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="5060" windowWidth="38400" windowHeight="22620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="5420" windowWidth="25460" windowHeight="21420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="412">
   <si>
     <t>id</t>
   </si>
@@ -1285,15 +1285,24 @@
   <si>
     <t>% not NA</t>
   </si>
+  <si>
+    <t>LoanStats Field</t>
+  </si>
+  <si>
+    <t>RejectStatsField</t>
+  </si>
+  <si>
+    <t>These matches are definitely not perfect (e.g. application date != issue date) but they're the best I can find.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1469,6 +1478,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1662,7 +1680,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1814,6 +1832,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1909,7 +1940,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1945,9 +1976,12 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2350,7 +2384,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A1:A2"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6777,9 +6811,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -6874,6 +6910,97 @@
     <row r="12" spans="1:2">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="str">
+        <f>A2</f>
+        <v>Amount Requested</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="str">
+        <f>A3</f>
+        <v>Application Date</v>
+      </c>
+      <c r="B15" s="11" t="str">
+        <f>LoanStats!A37</f>
+        <v>issue_d</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="str">
+        <f>A4</f>
+        <v>Loan Title</v>
+      </c>
+      <c r="B16" s="11" t="str">
+        <f>LoanStats!A97</f>
+        <v>title</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="str">
+        <f>A5</f>
+        <v>Risk_Score</v>
+      </c>
+      <c r="B17" s="11" t="str">
+        <f>LoanStats!A24</f>
+        <v>fico_range_low</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="str">
+        <f>A6</f>
+        <v>Debt-To-Income Ratio</v>
+      </c>
+      <c r="B18" s="11" t="str">
+        <f>LoanStats!A21</f>
+        <v>emp_length</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="str">
+        <f>A7</f>
+        <v>Zip Code</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="str">
+        <f>A8</f>
+        <v>State</v>
+      </c>
+      <c r="B20" s="11" t="str">
+        <f>LoanStats!A4</f>
+        <v>addr_state</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="str">
+        <f>A9</f>
+        <v>Employment Length</v>
+      </c>
+      <c r="B21" s="11" t="str">
+        <f>LoanStats!A21</f>
+        <v>emp_length</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="30" t="s">
+        <v>411</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -6930,7 +7057,7 @@
         <v>388</v>
       </c>
       <c r="E2" s="25">
-        <f>C2/2260701</f>
+        <f t="shared" ref="E2:E33" si="0">C2/2260701</f>
         <v>1</v>
       </c>
       <c r="F2" t="b">
@@ -6951,7 +7078,7 @@
         <v>389</v>
       </c>
       <c r="E3" s="25">
-        <f>C3/2260701</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6969,7 +7096,7 @@
         <v>389</v>
       </c>
       <c r="E4" s="25">
-        <f>C4/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -6987,7 +7114,7 @@
         <v>389</v>
       </c>
       <c r="E5" s="25">
-        <f>C5/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7005,7 +7132,7 @@
         <v>389</v>
       </c>
       <c r="E6" s="25">
-        <f>C6/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7023,7 +7150,7 @@
         <v>388</v>
       </c>
       <c r="E7" s="25">
-        <f>C7/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7041,7 +7168,7 @@
         <v>389</v>
       </c>
       <c r="E8" s="25">
-        <f>C8/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7059,7 +7186,7 @@
         <v>389</v>
       </c>
       <c r="E9" s="25">
-        <f>C9/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7077,7 +7204,7 @@
         <v>388</v>
       </c>
       <c r="E10" s="25">
-        <f>C10/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7095,7 +7222,7 @@
         <v>388</v>
       </c>
       <c r="E11" s="25">
-        <f>C11/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7113,7 +7240,7 @@
         <v>388</v>
       </c>
       <c r="E12" s="25">
-        <f>C12/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.92612822306001541</v>
       </c>
     </row>
@@ -7131,7 +7258,7 @@
         <v>388</v>
       </c>
       <c r="E13" s="25">
-        <f>C13/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.93500246162584089</v>
       </c>
     </row>
@@ -7149,7 +7276,7 @@
         <v>388</v>
       </c>
       <c r="E14" s="25">
-        <f>C14/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7167,7 +7294,7 @@
         <v>389</v>
       </c>
       <c r="E15" s="25">
-        <f>C15/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.9999836333951283</v>
       </c>
     </row>
@@ -7185,7 +7312,7 @@
         <v>388</v>
       </c>
       <c r="E16" s="25">
-        <f>C16/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7203,7 +7330,7 @@
         <v>388</v>
       </c>
       <c r="E17" s="25">
-        <f>C17/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7221,7 +7348,7 @@
         <v>388</v>
       </c>
       <c r="E18" s="25">
-        <f>C18/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7239,7 +7366,7 @@
         <v>388</v>
       </c>
       <c r="E19" s="25">
-        <f>C19/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7257,7 +7384,7 @@
         <v>388</v>
       </c>
       <c r="E20" s="25">
-        <f>C20/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7275,7 +7402,7 @@
         <v>388</v>
       </c>
       <c r="E21" s="25">
-        <f>C21/2260701</f>
+        <f t="shared" si="0"/>
         <v>5.5764561523173564E-2</v>
       </c>
       <c r="F21" t="b">
@@ -7296,7 +7423,7 @@
         <v>388</v>
       </c>
       <c r="E22" s="25">
-        <f>C22/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7314,7 +7441,7 @@
         <v>388</v>
       </c>
       <c r="E23" s="25">
-        <f>C23/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.98966780657857889</v>
       </c>
     </row>
@@ -7332,7 +7459,7 @@
         <v>388</v>
       </c>
       <c r="E24" s="25">
-        <f>C24/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998496041714491</v>
       </c>
     </row>
@@ -7350,7 +7477,7 @@
         <v>388</v>
       </c>
       <c r="E25" s="25">
-        <f>C25/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7368,7 +7495,7 @@
         <v>389</v>
       </c>
       <c r="E26" s="25">
-        <f>C26/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99922855786767029</v>
       </c>
     </row>
@@ -7386,7 +7513,7 @@
         <v>389</v>
       </c>
       <c r="E27" s="25">
-        <f>C27/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99997257487832314</v>
       </c>
     </row>
@@ -7404,7 +7531,7 @@
         <v>388</v>
       </c>
       <c r="E28" s="25">
-        <f>C28/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99997257487832314</v>
       </c>
     </row>
@@ -7422,7 +7549,7 @@
         <v>389</v>
       </c>
       <c r="E29" s="25">
-        <f>C29/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7440,7 +7567,7 @@
         <v>389</v>
       </c>
       <c r="E30" s="25">
-        <f>C30/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7458,7 +7585,7 @@
         <v>389</v>
       </c>
       <c r="E31" s="25">
-        <f>C31/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.99997213253765094</v>
       </c>
     </row>
@@ -7476,7 +7603,7 @@
         <v>389</v>
       </c>
       <c r="E32" s="25">
-        <f>C32/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.48753284932416979</v>
       </c>
     </row>
@@ -7494,7 +7621,7 @@
         <v>389</v>
       </c>
       <c r="E33" s="25">
-        <f>C33/2260701</f>
+        <f t="shared" si="0"/>
         <v>0.15886930646733027</v>
       </c>
     </row>
@@ -7512,7 +7639,7 @@
         <v>389</v>
       </c>
       <c r="E34" s="25">
-        <f>C34/2260701</f>
+        <f t="shared" ref="E34:E65" si="1">C34/2260701</f>
         <v>0.99997257487832314</v>
       </c>
     </row>
@@ -7530,7 +7657,7 @@
         <v>389</v>
       </c>
       <c r="E35" s="25">
-        <f>C35/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99997257487832314</v>
       </c>
     </row>
@@ -7548,7 +7675,7 @@
         <v>389</v>
       </c>
       <c r="E36" s="25">
-        <f>C36/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7566,7 +7693,7 @@
         <v>389</v>
       </c>
       <c r="E37" s="25">
-        <f>C37/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99918830486649934</v>
       </c>
     </row>
@@ -7584,7 +7711,7 @@
         <v>389</v>
       </c>
       <c r="E38" s="25">
-        <f>C38/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99997257487832314</v>
       </c>
     </row>
@@ -7602,7 +7729,7 @@
         <v>388</v>
       </c>
       <c r="E39" s="25">
-        <f>C39/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7620,7 +7747,7 @@
         <v>389</v>
       </c>
       <c r="E40" s="25">
-        <f>C40/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7638,7 +7765,7 @@
         <v>389</v>
       </c>
       <c r="E41" s="25">
-        <f>C41/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7656,7 +7783,7 @@
         <v>389</v>
       </c>
       <c r="E42" s="25">
-        <f>C42/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7674,7 +7801,7 @@
         <v>389</v>
       </c>
       <c r="E43" s="25">
-        <f>C43/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7692,7 +7819,7 @@
         <v>389</v>
       </c>
       <c r="E44" s="25">
-        <f>C44/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7710,7 +7837,7 @@
         <v>389</v>
       </c>
       <c r="E45" s="25">
-        <f>C45/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7728,7 +7855,7 @@
         <v>389</v>
       </c>
       <c r="E46" s="25">
-        <f>C46/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7746,7 +7873,7 @@
         <v>389</v>
       </c>
       <c r="E47" s="25">
-        <f>C47/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7764,7 +7891,7 @@
         <v>389</v>
       </c>
       <c r="E48" s="25">
-        <f>C48/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7782,7 +7909,7 @@
         <v>388</v>
       </c>
       <c r="E49" s="25">
-        <f>C49/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99891184194636973</v>
       </c>
     </row>
@@ -7800,7 +7927,7 @@
         <v>389</v>
       </c>
       <c r="E50" s="25">
-        <f>C50/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7818,7 +7945,7 @@
         <v>388</v>
       </c>
       <c r="E51" s="25">
-        <f>C51/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.40490007303044501</v>
       </c>
       <c r="F51" t="b">
@@ -7839,7 +7966,7 @@
         <v>388</v>
       </c>
       <c r="E52" s="25">
-        <f>C52/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99995355422941823</v>
       </c>
     </row>
@@ -7857,7 +7984,7 @@
         <v>389</v>
       </c>
       <c r="E53" s="25">
-        <f>C53/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7875,7 +8002,7 @@
         <v>389</v>
       </c>
       <c r="E54" s="25">
-        <f>C54/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7893,7 +8020,7 @@
         <v>389</v>
       </c>
       <c r="E55" s="25">
-        <f>C55/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99992126336034703</v>
       </c>
     </row>
@@ -7911,7 +8038,7 @@
         <v>389</v>
       </c>
       <c r="E56" s="25">
-        <f>C56/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.25690040390126778</v>
       </c>
     </row>
@@ -7929,7 +8056,7 @@
         <v>389</v>
       </c>
       <c r="E57" s="25">
-        <f>C57/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7947,7 +8074,7 @@
         <v>388</v>
       </c>
       <c r="E58" s="25">
-        <f>C58/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -7965,7 +8092,7 @@
         <v>389</v>
       </c>
       <c r="E59" s="25">
-        <f>C59/2260701</f>
+        <f t="shared" si="1"/>
         <v>5.3394942542158381E-2</v>
       </c>
     </row>
@@ -7983,7 +8110,7 @@
         <v>389</v>
       </c>
       <c r="E60" s="25">
-        <f>C60/2260701</f>
+        <f t="shared" si="1"/>
         <v>5.3393173179469552E-2</v>
       </c>
     </row>
@@ -8001,7 +8128,7 @@
         <v>388</v>
       </c>
       <c r="E61" s="25">
-        <f>C61/2260701</f>
+        <f t="shared" si="1"/>
         <v>5.1192085994565401E-2</v>
       </c>
       <c r="F61" t="b">
@@ -8022,7 +8149,7 @@
         <v>389</v>
       </c>
       <c r="E62" s="25">
-        <f>C62/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.99997257487832314</v>
       </c>
     </row>
@@ -8040,7 +8167,7 @@
         <v>389</v>
       </c>
       <c r="E63" s="25">
-        <f>C63/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8058,7 +8185,7 @@
         <v>389</v>
       </c>
       <c r="E64" s="25">
-        <f>C64/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8076,7 +8203,7 @@
         <v>389</v>
       </c>
       <c r="E65" s="25">
-        <f>C65/2260701</f>
+        <f t="shared" si="1"/>
         <v>0.61686087633879938</v>
       </c>
     </row>
@@ -8094,7 +8221,7 @@
         <v>389</v>
       </c>
       <c r="E66" s="25">
-        <f>C66/2260701</f>
+        <f t="shared" ref="E66:E97" si="2">C66/2260701</f>
         <v>0.61686131867947158</v>
       </c>
     </row>
@@ -8112,7 +8239,7 @@
         <v>389</v>
       </c>
       <c r="E67" s="25">
-        <f>C67/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.61686131867947158</v>
       </c>
     </row>
@@ -8130,7 +8257,7 @@
         <v>389</v>
       </c>
       <c r="E68" s="25">
-        <f>C68/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.61686131867947158</v>
       </c>
     </row>
@@ -8148,7 +8275,7 @@
         <v>389</v>
       </c>
       <c r="E69" s="25">
-        <f>C69/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.59748900894014734</v>
       </c>
     </row>
@@ -8166,7 +8293,7 @@
         <v>389</v>
       </c>
       <c r="E70" s="25">
-        <f>C70/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.61686131867947158</v>
       </c>
     </row>
@@ -8184,7 +8311,7 @@
         <v>389</v>
       </c>
       <c r="E71" s="25">
-        <f>C71/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.52718957526890997</v>
       </c>
     </row>
@@ -8202,7 +8329,7 @@
         <v>389</v>
       </c>
       <c r="E72" s="25">
-        <f>C72/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.61686131867947158</v>
       </c>
     </row>
@@ -8220,7 +8347,7 @@
         <v>389</v>
       </c>
       <c r="E73" s="25">
-        <f>C73/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.61686131867947158</v>
       </c>
     </row>
@@ -8238,7 +8365,7 @@
         <v>389</v>
       </c>
       <c r="E74" s="25">
-        <f>C74/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.61686131867947158</v>
       </c>
     </row>
@@ -8256,7 +8383,7 @@
         <v>389</v>
       </c>
       <c r="E75" s="25">
-        <f>C75/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.61676444607225811</v>
       </c>
     </row>
@@ -8274,7 +8401,7 @@
         <v>389</v>
       </c>
       <c r="E76" s="25">
-        <f>C76/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8292,7 +8419,7 @@
         <v>389</v>
       </c>
       <c r="E77" s="25">
-        <f>C77/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.61686131867947158</v>
       </c>
     </row>
@@ -8310,7 +8437,7 @@
         <v>389</v>
       </c>
       <c r="E78" s="25">
-        <f>C78/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.61686087633879938</v>
       </c>
     </row>
@@ -8328,7 +8455,7 @@
         <v>389</v>
       </c>
       <c r="E79" s="25">
-        <f>C79/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.61686087633879938</v>
       </c>
     </row>
@@ -8346,7 +8473,7 @@
         <v>389</v>
       </c>
       <c r="E80" s="25">
-        <f>C80/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.97785509892727962</v>
       </c>
     </row>
@@ -8364,7 +8491,7 @@
         <v>389</v>
       </c>
       <c r="E81" s="25">
-        <f>C81/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.9688685058307136</v>
       </c>
     </row>
@@ -8382,7 +8509,7 @@
         <v>389</v>
       </c>
       <c r="E82" s="25">
-        <f>C82/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.96683860448595371</v>
       </c>
     </row>
@@ -8400,7 +8527,7 @@
         <v>389</v>
       </c>
       <c r="E83" s="25">
-        <f>C83/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.96633610548232607</v>
       </c>
     </row>
@@ -8418,7 +8545,7 @@
         <v>389</v>
       </c>
       <c r="E84" s="25">
-        <f>C84/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.99992126336034703</v>
       </c>
     </row>
@@ -8436,7 +8563,7 @@
         <v>389</v>
       </c>
       <c r="E85" s="25">
-        <f>C85/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.99997257487832314</v>
       </c>
     </row>
@@ -8454,7 +8581,7 @@
         <v>389</v>
       </c>
       <c r="E86" s="25">
-        <f>C86/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.93846864313325817</v>
       </c>
     </row>
@@ -8472,7 +8599,7 @@
         <v>389</v>
       </c>
       <c r="E87" s="25">
-        <f>C87/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.96889902733709588</v>
       </c>
     </row>
@@ -8490,7 +8617,7 @@
         <v>389</v>
       </c>
       <c r="E88" s="25">
-        <f>C88/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.96889902733709588</v>
       </c>
     </row>
@@ -8508,7 +8635,7 @@
         <v>389</v>
       </c>
       <c r="E89" s="25">
-        <f>C89/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8526,7 +8653,7 @@
         <v>389</v>
       </c>
       <c r="E90" s="25">
-        <f>C90/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.97785509892727962</v>
       </c>
     </row>
@@ -8544,7 +8671,7 @@
         <v>389</v>
       </c>
       <c r="E91" s="25">
-        <f>C91/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.96751228932972555</v>
       </c>
     </row>
@@ -8562,7 +8689,7 @@
         <v>389</v>
       </c>
       <c r="E92" s="25">
-        <f>C92/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.22988488968687146</v>
       </c>
     </row>
@@ -8580,7 +8707,7 @@
         <v>389</v>
       </c>
       <c r="E93" s="25">
-        <f>C93/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.86930248626421625</v>
       </c>
     </row>
@@ -8598,7 +8725,7 @@
         <v>389</v>
       </c>
       <c r="E94" s="25">
-        <f>C94/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.32749089773481765</v>
       </c>
     </row>
@@ -8616,7 +8743,7 @@
         <v>389</v>
       </c>
       <c r="E95" s="25">
-        <f>C95/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8634,7 +8761,7 @@
         <v>389</v>
       </c>
       <c r="E96" s="25">
-        <f>C96/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8652,7 +8779,7 @@
         <v>389</v>
       </c>
       <c r="E97" s="25">
-        <f>C97/2260701</f>
+        <f t="shared" si="2"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8670,7 +8797,7 @@
         <v>389</v>
       </c>
       <c r="E98" s="25">
-        <f>C98/2260701</f>
+        <f t="shared" ref="E98:E129" si="3">C98/2260701</f>
         <v>0.97406866277318405</v>
       </c>
     </row>
@@ -8688,7 +8815,7 @@
         <v>389</v>
       </c>
       <c r="E99" s="25">
-        <f>C99/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8706,7 +8833,7 @@
         <v>389</v>
       </c>
       <c r="E100" s="25">
-        <f>C100/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8724,7 +8851,7 @@
         <v>389</v>
       </c>
       <c r="E101" s="25">
-        <f>C101/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8742,7 +8869,7 @@
         <v>389</v>
       </c>
       <c r="E102" s="25">
-        <f>C102/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96889902733709588</v>
       </c>
     </row>
@@ -8760,7 +8887,7 @@
         <v>389</v>
       </c>
       <c r="E103" s="25">
-        <f>C103/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8778,7 +8905,7 @@
         <v>389</v>
       </c>
       <c r="E104" s="25">
-        <f>C104/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.97406866277318405</v>
       </c>
     </row>
@@ -8796,7 +8923,7 @@
         <v>389</v>
       </c>
       <c r="E105" s="25">
-        <f>C105/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.93201666208844069</v>
       </c>
     </row>
@@ -8814,7 +8941,7 @@
         <v>389</v>
       </c>
       <c r="E106" s="25">
-        <f>C106/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8832,7 +8959,7 @@
         <v>389</v>
       </c>
       <c r="E107" s="25">
-        <f>C107/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8850,7 +8977,7 @@
         <v>389</v>
       </c>
       <c r="E108" s="25">
-        <f>C108/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8868,7 +8995,7 @@
         <v>389</v>
       </c>
       <c r="E109" s="25">
-        <f>C109/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96883090687357598</v>
       </c>
     </row>
@@ -8886,7 +9013,7 @@
         <v>389</v>
       </c>
       <c r="E110" s="25">
-        <f>C110/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96664220522749356</v>
       </c>
     </row>
@@ -8904,7 +9031,7 @@
         <v>389</v>
       </c>
       <c r="E111" s="25">
-        <f>C111/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.99938160774025397</v>
       </c>
     </row>
@@ -8922,7 +9049,7 @@
         <v>389</v>
       </c>
       <c r="E112" s="25">
-        <f>C112/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.99993895698723534</v>
       </c>
     </row>
@@ -8940,7 +9067,7 @@
         <v>389</v>
       </c>
       <c r="E113" s="25">
-        <f>C113/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -8958,7 +9085,7 @@
         <v>389</v>
       </c>
       <c r="E114" s="25">
-        <f>C114/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.97785509892727962</v>
       </c>
     </row>
@@ -8976,7 +9103,7 @@
         <v>389</v>
       </c>
       <c r="E115" s="25">
-        <f>C115/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.97785509892727962</v>
       </c>
     </row>
@@ -8994,7 +9121,7 @@
         <v>389</v>
       </c>
       <c r="E116" s="25">
-        <f>C116/2260701</f>
+        <f t="shared" si="3"/>
         <v>0.96889946967776808</v>
       </c>
     </row>
@@ -9012,7 +9139,7 @@
         <v>389</v>
       </c>
       <c r="E117" s="25">
-        <f>C117/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.7781639411846148E-2</v>
       </c>
     </row>
@@ -9030,7 +9157,7 @@
         <v>389</v>
       </c>
       <c r="E118" s="25">
-        <f>C118/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.7782081752518357E-2</v>
       </c>
     </row>
@@ -9048,7 +9175,7 @@
         <v>389</v>
       </c>
       <c r="E119" s="25">
-        <f>C119/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.7782081752518357E-2</v>
       </c>
     </row>
@@ -9066,7 +9193,7 @@
         <v>388</v>
       </c>
       <c r="E120" s="25">
-        <f>C120/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.7782081752518357E-2</v>
       </c>
       <c r="F120" t="b">
@@ -9087,7 +9214,7 @@
         <v>389</v>
       </c>
       <c r="E121" s="25">
-        <f>C121/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.7782081752518357E-2</v>
       </c>
     </row>
@@ -9105,7 +9232,7 @@
         <v>389</v>
       </c>
       <c r="E122" s="25">
-        <f>C122/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.7782081752518357E-2</v>
       </c>
     </row>
@@ -9123,7 +9250,7 @@
         <v>389</v>
       </c>
       <c r="E123" s="25">
-        <f>C123/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.7782081752518357E-2</v>
       </c>
     </row>
@@ -9141,7 +9268,7 @@
         <v>389</v>
       </c>
       <c r="E124" s="25">
-        <f>C124/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.6969501937673318E-2</v>
       </c>
     </row>
@@ -9159,7 +9286,7 @@
         <v>389</v>
       </c>
       <c r="E125" s="25">
-        <f>C125/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.7782081752518357E-2</v>
       </c>
     </row>
@@ -9177,7 +9304,7 @@
         <v>389</v>
       </c>
       <c r="E126" s="25">
-        <f>C126/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.7782081752518357E-2</v>
       </c>
     </row>
@@ -9195,7 +9322,7 @@
         <v>389</v>
       </c>
       <c r="E127" s="25">
-        <f>C127/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.7782081752518357E-2</v>
       </c>
     </row>
@@ -9213,7 +9340,7 @@
         <v>389</v>
       </c>
       <c r="E128" s="25">
-        <f>C128/2260701</f>
+        <f t="shared" si="3"/>
         <v>4.7782081752518357E-2</v>
       </c>
     </row>
@@ -9231,7 +9358,7 @@
         <v>389</v>
       </c>
       <c r="E129" s="25">
-        <f>C129/2260701</f>
+        <f t="shared" si="3"/>
         <v>1.5898608440479304E-2</v>
       </c>
     </row>
@@ -9249,7 +9376,7 @@
         <v>388</v>
       </c>
       <c r="E130" s="25">
-        <f>C130/2260701</f>
+        <f t="shared" ref="E130:E152" si="4">C130/2260701</f>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -9267,7 +9394,7 @@
         <v>388</v>
       </c>
       <c r="E131" s="25">
-        <f>C131/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
       <c r="F131" t="b">
@@ -9288,7 +9415,7 @@
         <v>388</v>
       </c>
       <c r="E132" s="25">
-        <f>C132/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
       <c r="F132" t="b">
@@ -9309,7 +9436,7 @@
         <v>388</v>
       </c>
       <c r="E133" s="25">
-        <f>C133/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
       <c r="F133" t="b">
@@ -9330,7 +9457,7 @@
         <v>389</v>
       </c>
       <c r="E134" s="25">
-        <f>C134/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
     </row>
@@ -9348,7 +9475,7 @@
         <v>389</v>
       </c>
       <c r="E135" s="25">
-        <f>C135/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
     </row>
@@ -9366,7 +9493,7 @@
         <v>388</v>
       </c>
       <c r="E136" s="25">
-        <f>C136/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
       <c r="F136" t="b">
@@ -9387,7 +9514,7 @@
         <v>388</v>
       </c>
       <c r="E137" s="25">
-        <f>C137/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
       <c r="F137" t="b">
@@ -9408,7 +9535,7 @@
         <v>388</v>
       </c>
       <c r="E138" s="25">
-        <f>C138/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
       <c r="F138" t="b">
@@ -9429,7 +9556,7 @@
         <v>389</v>
       </c>
       <c r="E139" s="25">
-        <f>C139/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
     </row>
@@ -9447,7 +9574,7 @@
         <v>389</v>
       </c>
       <c r="E140" s="25">
-        <f>C140/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
     </row>
@@ -9465,7 +9592,7 @@
         <v>388</v>
       </c>
       <c r="E141" s="25">
-        <f>C141/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
       <c r="F141" t="b">
@@ -9486,7 +9613,7 @@
         <v>389</v>
       </c>
       <c r="E142" s="25">
-        <f>C142/2260701</f>
+        <f t="shared" si="4"/>
         <v>3.8266891552664415E-3</v>
       </c>
     </row>
@@ -9504,7 +9631,7 @@
         <v>389</v>
       </c>
       <c r="E143" s="25">
-        <f>C143/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
     </row>
@@ -9522,7 +9649,7 @@
         <v>389</v>
       </c>
       <c r="E144" s="25">
-        <f>C144/2260701</f>
+        <f t="shared" si="4"/>
         <v>4.829033118488469E-3</v>
       </c>
     </row>
@@ -9540,7 +9667,7 @@
         <v>388</v>
       </c>
       <c r="E145" s="25">
-        <f>C145/2260701</f>
+        <f t="shared" si="4"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -9558,7 +9685,7 @@
         <v>388</v>
       </c>
       <c r="E146" s="25">
-        <f>C146/2260701</f>
+        <f t="shared" si="4"/>
         <v>0.99998540275781711</v>
       </c>
     </row>
@@ -9576,7 +9703,7 @@
         <v>388</v>
       </c>
       <c r="E147" s="25">
-        <f>C147/2260701</f>
+        <f t="shared" si="4"/>
         <v>1.5148398660415507E-2</v>
       </c>
       <c r="F147" t="b">
@@ -9597,7 +9724,7 @@
         <v>388</v>
       </c>
       <c r="E148" s="25">
-        <f>C148/2260701</f>
+        <f t="shared" si="4"/>
         <v>1.5148398660415507E-2</v>
       </c>
       <c r="F148" t="b">
@@ -9618,7 +9745,7 @@
         <v>388</v>
       </c>
       <c r="E149" s="25">
-        <f>C149/2260701</f>
+        <f t="shared" si="4"/>
         <v>1.5148398660415507E-2</v>
       </c>
       <c r="F149" t="b">
@@ -9639,7 +9766,7 @@
         <v>389</v>
       </c>
       <c r="E150" s="25">
-        <f>C150/2260701</f>
+        <f t="shared" si="4"/>
         <v>1.5148398660415507E-2</v>
       </c>
     </row>
@@ -9657,7 +9784,7 @@
         <v>389</v>
       </c>
       <c r="E151" s="25">
-        <f>C151/2260701</f>
+        <f t="shared" si="4"/>
         <v>1.5148398660415507E-2</v>
       </c>
     </row>
@@ -9675,7 +9802,7 @@
         <v>389</v>
       </c>
       <c r="E152" s="25">
-        <f>C152/2260701</f>
+        <f t="shared" si="4"/>
         <v>1.5148398660415507E-2</v>
       </c>
     </row>

</xml_diff>